<commit_message>
modif narratif index (#133)
* modif narratif index

* Update input/pagecontent/index.md

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

---------

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> afeefda3edd13a9cd98c23042a7a42d64cb8b1ea
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-eclaire-group-characteristic-kind-code-system.xlsx
+++ b/main/ig/CodeSystem-eclaire-group-characteristic-kind-code-system.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.3.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-14T09:59:11+00:00</t>
+    <t>2024-03-14T13:53:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>